<commit_message>
updating stats with new ecotaxa data
</commit_message>
<xml_diff>
--- a/Data/Diversity_wider.xlsx
+++ b/Data/Diversity_wider.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -490,13 +490,13 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>1606</v>
+        <v>1602</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -562,10 +562,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -634,13 +634,13 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G4">
-        <v>2966</v>
+        <v>2973</v>
       </c>
       <c r="H4">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="I4">
         <v>13</v>
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>3775</v>
+        <v>3757</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -706,16 +706,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G5">
-        <v>723</v>
+        <v>750</v>
       </c>
       <c r="H5">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>8647</v>
+        <v>8631</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -751,7 +751,7 @@
         <v>2</v>
       </c>
       <c r="U5">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -778,13 +778,13 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G6">
-        <v>936</v>
+        <v>951</v>
       </c>
       <c r="H6">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="I6">
         <v>7</v>
@@ -793,10 +793,10 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>6447</v>
+        <v>6431</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -820,10 +820,10 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U6">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1069,13 +1069,13 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1141,7 +1141,7 @@
         <v>4</v>
       </c>
       <c r="G11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1213,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1327,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -1426,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1459,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1329</v>
+        <v>1335</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="U17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -1675,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1687,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="U18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -1714,10 +1714,10 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1786,13 +1786,13 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G20">
-        <v>473</v>
+        <v>491</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="Q20">
-        <v>5668</v>
+        <v>5654</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -1828,10 +1828,10 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U20">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -1858,16 +1858,16 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G21">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="H21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>4907</v>
+        <v>4923</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -1930,16 +1930,16 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G22">
-        <v>631</v>
+        <v>649</v>
       </c>
       <c r="H22">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I22">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1948,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -1963,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>5198</v>
+        <v>5179</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -1975,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="U22">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -2002,13 +2002,13 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G23">
-        <v>1600</v>
+        <v>1621</v>
       </c>
       <c r="H23">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I23">
         <v>14</v>
@@ -2017,10 +2017,10 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -2035,22 +2035,22 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>9909</v>
+        <v>9896</v>
       </c>
       <c r="R23">
         <v>1</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U23">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="V23">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2074,22 +2074,22 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G24">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
         <v>20</v>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="U24">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V24">
         <v>1</v>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2149,13 +2149,13 @@
         <v>96</v>
       </c>
       <c r="G25">
-        <v>578</v>
+        <v>587</v>
       </c>
       <c r="H25">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -2164,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2179,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>5924</v>
+        <v>5914</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="U25">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="V25">
         <v>0</v>
@@ -2218,16 +2218,16 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G26">
-        <v>745</v>
+        <v>761</v>
       </c>
       <c r="H26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>11528</v>
+        <v>11516</v>
       </c>
       <c r="R26">
         <v>0</v>
@@ -2260,10 +2260,10 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U26">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="V26">
         <v>0</v>
@@ -2284,16 +2284,16 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="R27">
         <v>0</v>
@@ -2335,7 +2335,7 @@
         <v>1</v>
       </c>
       <c r="U27">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -2362,13 +2362,13 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G28">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I28">
         <v>2</v>
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="R28">
         <v>0</v>
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="U28">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -2437,7 +2437,7 @@
         <v>9</v>
       </c>
       <c r="G29">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2467,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -2479,7 +2479,7 @@
         <v>0</v>
       </c>
       <c r="U29">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -2506,13 +2506,13 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G30">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="H30">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="L30">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -2539,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <v>7882</v>
+        <v>7877</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -2548,10 +2548,10 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U30">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -2581,7 +2581,7 @@
         <v>10</v>
       </c>
       <c r="G31">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H31">
         <v>2</v>
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="R31">
         <v>0</v>
@@ -2623,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="U31">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="V31">
         <v>0</v>
@@ -2650,13 +2650,13 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G32">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2683,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -2695,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="U32">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -2725,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="G33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -2764,10 +2764,10 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U33">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -2794,16 +2794,16 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="L34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="U34">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -2866,10 +2866,10 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G35">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="Q35">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="R35">
         <v>0</v>
@@ -2911,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="U35">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V35">
         <v>0</v>
@@ -2941,7 +2941,7 @@
         <v>4</v>
       </c>
       <c r="G36">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="R36">
         <v>0</v>
@@ -3013,7 +3013,7 @@
         <v>3</v>
       </c>
       <c r="G37">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="L37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -3043,7 +3043,7 @@
         <v>0</v>
       </c>
       <c r="Q37">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="R37">
         <v>0</v>
@@ -3082,16 +3082,16 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="G38">
-        <v>864</v>
+        <v>885</v>
       </c>
       <c r="H38">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -3115,7 +3115,7 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>14223</v>
+        <v>14209</v>
       </c>
       <c r="R38">
         <v>0</v>
@@ -3127,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="U38">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="V38">
         <v>0</v>
@@ -3154,13 +3154,13 @@
         <v>14</v>
       </c>
       <c r="F39">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39">
         <v>89</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <v>1438</v>
+        <v>1440</v>
       </c>
       <c r="R39">
         <v>0</v>
@@ -3199,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="U39">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V39">
         <v>0</v>
@@ -3226,13 +3226,13 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G40">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="H40">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I40">
         <v>8</v>
@@ -3244,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="L40">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M40">
         <v>0</v>
@@ -3259,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>5889</v>
+        <v>5874</v>
       </c>
       <c r="R40">
         <v>0</v>
@@ -3271,10 +3271,10 @@
         <v>0</v>
       </c>
       <c r="U40">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -3298,16 +3298,16 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G41">
         <v>501</v>
       </c>
       <c r="H41">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I41">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -3316,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="L41">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M41">
         <v>0</v>
@@ -3331,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>3857</v>
+        <v>3855</v>
       </c>
       <c r="R41">
         <v>0</v>
@@ -3370,16 +3370,16 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G42">
-        <v>999</v>
+        <v>1006</v>
       </c>
       <c r="H42">
         <v>19</v>
       </c>
       <c r="I42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -3388,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="L42">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -3403,7 +3403,7 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <v>12995</v>
+        <v>12999</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -3412,19 +3412,19 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U42">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="V42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>JL_June_Henry</t>
+          <t>JL_August_Henry</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3442,16 +3442,16 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="G43">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="H43">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="L43">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="M43">
         <v>0</v>
@@ -3472,31 +3472,31 @@
         <v>0</v>
       </c>
       <c r="P43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q43">
-        <v>5208</v>
+        <v>4609</v>
       </c>
       <c r="R43">
         <v>0</v>
       </c>
       <c r="S43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T43">
         <v>0</v>
       </c>
       <c r="U43">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="V43">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>OLA1_May_Henry</t>
+          <t>JL_June_Henry</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3514,16 +3514,16 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="G44">
-        <v>12</v>
+        <v>642</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -3532,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -3547,10 +3547,10 @@
         <v>0</v>
       </c>
       <c r="Q44">
-        <v>126</v>
+        <v>5186</v>
       </c>
       <c r="R44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S44">
         <v>0</v>
@@ -3559,16 +3559,16 @@
         <v>0</v>
       </c>
       <c r="U44">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="V44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>OLA2_May_Henry</t>
+          <t>OLA1_May_Henry</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3586,52 +3586,52 @@
         <v>0</v>
       </c>
       <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>126</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
         <v>6</v>
-      </c>
-      <c r="G45">
-        <v>18</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-      <c r="P45">
-        <v>0</v>
-      </c>
-      <c r="Q45">
-        <v>350</v>
-      </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
-      <c r="S45">
-        <v>0</v>
-      </c>
-      <c r="T45">
-        <v>0</v>
-      </c>
-      <c r="U45">
-        <v>19</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -3640,7 +3640,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>OLA3_May_Henry</t>
+          <t>OLA2_May_Henry</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3658,13 +3658,13 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G46">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <v>138</v>
+        <v>351</v>
       </c>
       <c r="R46">
         <v>0</v>
@@ -3703,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="U46">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="V46">
         <v>0</v>
@@ -3712,7 +3712,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>OLB1_May_Henry</t>
+          <t>OLA3_May_Henry</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3733,10 +3733,10 @@
         <v>2</v>
       </c>
       <c r="G47">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -3748,7 +3748,7 @@
         <v>0</v>
       </c>
       <c r="L47">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>420</v>
+        <v>139</v>
       </c>
       <c r="R47">
         <v>0</v>
@@ -3775,7 +3775,7 @@
         <v>0</v>
       </c>
       <c r="U47">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="V47">
         <v>0</v>
@@ -3784,7 +3784,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>OLB2_May_Henry</t>
+          <t>OLB1_May_Henry</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3802,26 +3802,26 @@
         <v>0</v>
       </c>
       <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>21</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
         <v>3</v>
       </c>
-      <c r="G48">
-        <v>15</v>
-      </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
       <c r="M48">
         <v>0</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="Q48">
-        <v>276</v>
+        <v>421</v>
       </c>
       <c r="R48">
         <v>0</v>
@@ -3847,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="U48">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V48">
         <v>0</v>
@@ -3856,7 +3856,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>OLB3_May_Henry</t>
+          <t>OLB2_May_Henry</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3877,10 +3877,10 @@
         <v>3</v>
       </c>
       <c r="G49">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -3892,7 +3892,7 @@
         <v>0</v>
       </c>
       <c r="L49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -3907,7 +3907,7 @@
         <v>0</v>
       </c>
       <c r="Q49">
-        <v>217</v>
+        <v>276</v>
       </c>
       <c r="R49">
         <v>0</v>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="U49">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V49">
         <v>0</v>
@@ -3928,7 +3928,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>OLC1_May_Henry</t>
+          <t>OLB3_May_Henry</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3946,13 +3946,13 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G50">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -3964,7 +3964,7 @@
         <v>0</v>
       </c>
       <c r="L50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -3979,7 +3979,7 @@
         <v>0</v>
       </c>
       <c r="Q50">
-        <v>322</v>
+        <v>217</v>
       </c>
       <c r="R50">
         <v>0</v>
@@ -3991,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="U50">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V50">
         <v>0</v>
@@ -4000,7 +4000,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>OLC2_May_Henry</t>
+          <t>OLC1_May_Henry</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4018,16 +4018,16 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -4036,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="L51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -4051,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="Q51">
-        <v>133</v>
+        <v>322</v>
       </c>
       <c r="R51">
         <v>0</v>
@@ -4060,10 +4060,10 @@
         <v>0</v>
       </c>
       <c r="T51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -4072,7 +4072,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>OLC3_May_Henry</t>
+          <t>OLC2_May_Henry</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4093,10 +4093,10 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -4123,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="Q52">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="R52">
         <v>0</v>
@@ -4135,7 +4135,7 @@
         <v>0</v>
       </c>
       <c r="U52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V52">
         <v>0</v>
@@ -4144,7 +4144,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>OLD1_May_Henry</t>
+          <t>OLC3_May_Henry</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4162,14 +4162,14 @@
         <v>0</v>
       </c>
       <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>9</v>
+      </c>
+      <c r="H53">
         <v>2</v>
       </c>
-      <c r="G53">
-        <v>6</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
       <c r="I53">
         <v>0</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="Q53">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="R53">
         <v>0</v>
@@ -4207,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="U53">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V53">
         <v>0</v>
@@ -4216,7 +4216,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>OLD2_May_Henry</t>
+          <t>OLD1_May_Henry</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4234,10 +4234,10 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -4252,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -4267,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="Q54">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="R54">
         <v>0</v>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="U54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -4288,7 +4288,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>OLD3_May_Henry</t>
+          <t>OLD2_May_Henry</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4306,10 +4306,10 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="Q55">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R55">
         <v>0</v>
@@ -4351,7 +4351,7 @@
         <v>0</v>
       </c>
       <c r="U55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V55">
         <v>0</v>
@@ -4360,7 +4360,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>OLE1_May_Henry</t>
+          <t>OLD3_May_Henry</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4378,52 +4378,52 @@
         <v>0</v>
       </c>
       <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>9</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>65</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <v>0</v>
+      </c>
+      <c r="U56">
         <v>3</v>
-      </c>
-      <c r="G56">
-        <v>8</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>1</v>
-      </c>
-      <c r="M56">
-        <v>0</v>
-      </c>
-      <c r="N56">
-        <v>0</v>
-      </c>
-      <c r="O56">
-        <v>0</v>
-      </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
-      <c r="Q56">
-        <v>160</v>
-      </c>
-      <c r="R56">
-        <v>0</v>
-      </c>
-      <c r="S56">
-        <v>0</v>
-      </c>
-      <c r="T56">
-        <v>0</v>
-      </c>
-      <c r="U56">
-        <v>7</v>
       </c>
       <c r="V56">
         <v>0</v>
@@ -4432,7 +4432,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>OLE2_May_Henry</t>
+          <t>OLE1_May_Henry</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4450,10 +4450,10 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G57">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -4468,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="L57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M57">
         <v>0</v>
@@ -4483,7 +4483,7 @@
         <v>0</v>
       </c>
       <c r="Q57">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="R57">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="U57">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="V57">
         <v>0</v>
@@ -4504,7 +4504,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>OLE3_May_Henry</t>
+          <t>OLE2_May_Henry</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4522,10 +4522,10 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G58">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4540,7 +4540,7 @@
         <v>0</v>
       </c>
       <c r="L58">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M58">
         <v>0</v>
@@ -4555,7 +4555,7 @@
         <v>0</v>
       </c>
       <c r="Q58">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R58">
         <v>0</v>
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="U58">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V58">
         <v>0</v>
@@ -4576,7 +4576,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>OLF1_May_Henry</t>
+          <t>OLE3_May_Henry</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4594,10 +4594,10 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -4612,34 +4612,34 @@
         <v>0</v>
       </c>
       <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>92</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59">
         <v>2</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
-      </c>
-      <c r="N59">
-        <v>0</v>
-      </c>
-      <c r="O59">
-        <v>0</v>
-      </c>
-      <c r="P59">
-        <v>0</v>
-      </c>
-      <c r="Q59">
-        <v>79</v>
-      </c>
-      <c r="R59">
-        <v>0</v>
-      </c>
-      <c r="S59">
-        <v>0</v>
-      </c>
-      <c r="T59">
-        <v>0</v>
-      </c>
-      <c r="U59">
-        <v>0</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -4648,7 +4648,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>OLF2_May_Henry</t>
+          <t>OLF1_May_Henry</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4666,26 +4666,26 @@
         <v>0</v>
       </c>
       <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>4</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
         <v>2</v>
       </c>
-      <c r="G60">
-        <v>2</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
       <c r="M60">
         <v>0</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>0</v>
       </c>
       <c r="Q60">
-        <v>136</v>
+        <v>77</v>
       </c>
       <c r="R60">
         <v>0</v>
@@ -4711,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="U60">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="V60">
         <v>0</v>
@@ -4720,7 +4720,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>OLF3_May_Henry</t>
+          <t>OLF2_May_Henry</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G61">
         <v>2</v>
@@ -4747,7 +4747,7 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -4756,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="L61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61">
         <v>0</v>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="Q61">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="R61">
         <v>0</v>
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="U61">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V61">
         <v>0</v>
@@ -4792,7 +4792,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>OL_July_Henry</t>
+          <t>OLF3_May_Henry</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4804,22 +4804,22 @@
         <v>0</v>
       </c>
       <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
         <v>2</v>
       </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>192</v>
-      </c>
-      <c r="G62">
-        <v>1235</v>
-      </c>
       <c r="H62">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="I62">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -4828,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="L62">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="M62">
         <v>0</v>
@@ -4843,28 +4843,28 @@
         <v>0</v>
       </c>
       <c r="Q62">
-        <v>17442</v>
+        <v>63</v>
       </c>
       <c r="R62">
         <v>0</v>
       </c>
       <c r="S62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T62">
         <v>0</v>
       </c>
       <c r="U62">
-        <v>892</v>
+        <v>1</v>
       </c>
       <c r="V62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SD1_May_Henry</t>
+          <t>OL_July_Henry</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4882,25 +4882,25 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>444</v>
+        <v>201</v>
       </c>
       <c r="G63">
-        <v>2389</v>
+        <v>1256</v>
       </c>
       <c r="H63">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="I63">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J63">
         <v>0</v>
       </c>
       <c r="K63">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L63">
-        <v>1666</v>
+        <v>236</v>
       </c>
       <c r="M63">
         <v>0</v>
@@ -4912,31 +4912,31 @@
         <v>0</v>
       </c>
       <c r="P63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q63">
-        <v>8851</v>
+        <v>17415</v>
       </c>
       <c r="R63">
         <v>0</v>
       </c>
       <c r="S63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U63">
-        <v>353</v>
+        <v>882</v>
       </c>
       <c r="V63">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SD2_May_Henry</t>
+          <t>SD1_May_Henry</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -4945,7 +4945,7 @@
         </is>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4954,25 +4954,25 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>276</v>
+        <v>439</v>
       </c>
       <c r="G64">
-        <v>2961</v>
+        <v>2384</v>
       </c>
       <c r="H64">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="I64">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J64">
         <v>0</v>
       </c>
       <c r="K64">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="L64">
-        <v>1458</v>
+        <v>1668</v>
       </c>
       <c r="M64">
         <v>0</v>
@@ -4987,7 +4987,7 @@
         <v>0</v>
       </c>
       <c r="Q64">
-        <v>2718</v>
+        <v>8858</v>
       </c>
       <c r="R64">
         <v>0</v>
@@ -4996,19 +4996,19 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U64">
-        <v>183</v>
+        <v>351</v>
       </c>
       <c r="V64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SD3_May_Henry</t>
+          <t>SD2_May_Henry</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5020,31 +5020,31 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <v>458</v>
+        <v>287</v>
       </c>
       <c r="G65">
-        <v>3029</v>
+        <v>2966</v>
       </c>
       <c r="H65">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I65">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="J65">
         <v>0</v>
       </c>
       <c r="K65">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L65">
-        <v>2059</v>
+        <v>1452</v>
       </c>
       <c r="M65">
         <v>0</v>
@@ -5059,7 +5059,7 @@
         <v>0</v>
       </c>
       <c r="Q65">
-        <v>12174</v>
+        <v>2714</v>
       </c>
       <c r="R65">
         <v>0</v>
@@ -5068,84 +5068,300 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U65">
-        <v>452</v>
+        <v>182</v>
       </c>
       <c r="V65">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>SD3_May_Henry</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>450</v>
+      </c>
+      <c r="G66">
+        <v>3041</v>
+      </c>
+      <c r="H66">
+        <v>126</v>
+      </c>
+      <c r="I66">
+        <v>17</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>8</v>
+      </c>
+      <c r="L66">
+        <v>2060</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>12186</v>
+      </c>
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>446</v>
+      </c>
+      <c r="V66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>SD_August_Henry</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>227</v>
+      </c>
+      <c r="G67">
+        <v>2707</v>
+      </c>
+      <c r="H67">
+        <v>88</v>
+      </c>
+      <c r="I67">
+        <v>5</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>5</v>
+      </c>
+      <c r="L67">
+        <v>870</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>1</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>7244</v>
+      </c>
+      <c r="R67">
+        <v>4</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+      <c r="T67">
+        <v>0</v>
+      </c>
+      <c r="U67">
+        <v>411</v>
+      </c>
+      <c r="V67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SD_July_Henry</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>524</v>
+      </c>
+      <c r="G68">
+        <v>1952</v>
+      </c>
+      <c r="H68">
+        <v>149</v>
+      </c>
+      <c r="I68">
+        <v>16</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>8</v>
+      </c>
+      <c r="L68">
+        <v>1680</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>11141</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68">
+        <v>1</v>
+      </c>
+      <c r="U68">
+        <v>467</v>
+      </c>
+      <c r="V68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>SD_September_Henry</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
         <v>53</v>
       </c>
-      <c r="F66">
-        <v>93</v>
-      </c>
-      <c r="G66">
-        <v>523</v>
-      </c>
-      <c r="H66">
-        <v>15</v>
-      </c>
-      <c r="I66">
-        <v>8</v>
-      </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
-        <v>48</v>
-      </c>
-      <c r="M66">
-        <v>0</v>
-      </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66">
-        <v>1</v>
-      </c>
-      <c r="P66">
-        <v>0</v>
-      </c>
-      <c r="Q66">
-        <v>6796</v>
-      </c>
-      <c r="R66">
-        <v>1</v>
-      </c>
-      <c r="S66">
-        <v>1</v>
-      </c>
-      <c r="T66">
-        <v>3</v>
-      </c>
-      <c r="U66">
-        <v>254</v>
-      </c>
-      <c r="V66">
+      <c r="F69">
+        <v>91</v>
+      </c>
+      <c r="G69">
+        <v>524</v>
+      </c>
+      <c r="H69">
+        <v>20</v>
+      </c>
+      <c r="I69">
+        <v>7</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>52</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>6780</v>
+      </c>
+      <c r="R69">
+        <v>1</v>
+      </c>
+      <c r="S69">
+        <v>1</v>
+      </c>
+      <c r="T69">
+        <v>6</v>
+      </c>
+      <c r="U69">
+        <v>259</v>
+      </c>
+      <c r="V69">
         <v>1</v>
       </c>
     </row>

</xml_diff>